<commit_message>
Update report and python script name
</commit_message>
<xml_diff>
--- a/Reports/Final Report Tables.xlsx
+++ b/Reports/Final Report Tables.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="416" documentId="8_{529A81D9-D3FF-4834-85A7-F5290A07351F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A9201C84-592C-491B-BE51-F57FBACD5ECB}"/>
   <bookViews>
-    <workbookView xWindow="825" yWindow="-120" windowWidth="37695" windowHeight="21840" xr2:uid="{9271DE90-5225-4E0F-95EF-B7F1D61D42E6}"/>
+    <workbookView xWindow="38280" yWindow="1635" windowWidth="38640" windowHeight="15840" xr2:uid="{9271DE90-5225-4E0F-95EF-B7F1D61D42E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Feature List" sheetId="1" r:id="rId1"/>
@@ -35,12 +35,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="73">
   <si>
     <t>Robotic Grasping - Feature List</t>
-  </si>
-  <si>
-    <t>Column1</t>
   </si>
   <si>
     <t>Feature No.</t>
@@ -275,14 +272,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -397,12 +387,11 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="18">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -413,31 +402,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -594,7 +584,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CACE4114-6C44-4F71-B0E2-9889E1826180}" name="Table1" displayName="Table1" ref="A3:G14" totalsRowShown="0" headerRowDxfId="12" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CACE4114-6C44-4F71-B0E2-9889E1826180}" name="Table1" displayName="Table1" ref="A3:G14" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <autoFilter ref="A3:G14" xr:uid="{17F19FCB-6C93-4847-B0AE-0ED9202CC537}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -605,13 +595,13 @@
     <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{F00FB1CD-463D-4194-B6BF-312CB80AE4E9}" name="Feature No." dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{A54A355A-AA23-4DDC-8871-773F493FE003}" name="Feature Name" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{9256D8FE-C049-4533-9F65-DF7C910707C0}" name="Summary" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{22075168-A916-49DC-884B-FD3EDE3BD5F1}" name="Complexity (1 - 5)" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{9A128FAD-94B2-4DF0-95F7-289C8AEBE228}" name="Iteration" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{CF15D37B-99DF-4EDE-BEAA-69E272604B88}" name="Completion" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{B467B4C0-BB3E-4E1C-B42E-873EAC231623}" name="Extra Details" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{F00FB1CD-463D-4194-B6BF-312CB80AE4E9}" name="Feature No." dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{A54A355A-AA23-4DDC-8871-773F493FE003}" name="Feature Name" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{9256D8FE-C049-4533-9F65-DF7C910707C0}" name="Summary" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{22075168-A916-49DC-884B-FD3EDE3BD5F1}" name="Complexity (1 - 5)" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{9A128FAD-94B2-4DF0-95F7-289C8AEBE228}" name="Iteration" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{CF15D37B-99DF-4EDE-BEAA-69E272604B88}" name="Completion" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{B467B4C0-BB3E-4E1C-B42E-873EAC231623}" name="Extra Details" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -968,8 +958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F98562E5-D21F-4DC0-9B50-01BAB35E5B7D}">
   <dimension ref="A1:Z14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -984,285 +974,285 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="2" t="s">
+    </row>
+    <row r="4" spans="1:26" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="3">
+        <v>3</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="3">
+        <v>3</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:26" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="3">
+        <v>2</v>
+      </c>
+      <c r="E6" s="3">
+        <v>2</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="T6" s="6"/>
+      <c r="U6" s="5"/>
+      <c r="V6" s="6"/>
+      <c r="W6" s="6"/>
+      <c r="X6" s="6"/>
+      <c r="Y6" s="6"/>
+      <c r="Z6" s="6"/>
+    </row>
+    <row r="7" spans="1:26" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>4</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:26" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+      <c r="C7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="3">
+        <v>2</v>
+      </c>
+      <c r="E7" s="3">
         <v>1</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="4">
+      <c r="F7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>5</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="3">
+        <v>4</v>
+      </c>
+      <c r="E8" s="3">
+        <v>2</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:26" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>6</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="3">
+        <v>5</v>
+      </c>
+      <c r="E9" s="3">
         <v>3</v>
       </c>
-      <c r="E4" s="4">
+      <c r="F9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>7</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="3">
+        <v>4</v>
+      </c>
+      <c r="E10" s="3">
+        <v>3</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>8</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="3">
+        <v>3</v>
+      </c>
+      <c r="E11" s="3">
+        <v>3</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>9</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="3">
+        <v>5</v>
+      </c>
+      <c r="E12" s="3">
+        <v>4</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="1:26" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>10</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="3">
+        <v>2</v>
+      </c>
+      <c r="E13" s="3">
+        <v>4</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:26" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>11</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="3">
         <v>1</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>2</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="4">
-        <v>3</v>
-      </c>
-      <c r="E5" s="4">
-        <v>1</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:26" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <v>3</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="4">
-        <v>2</v>
-      </c>
-      <c r="E6" s="4">
-        <v>2</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="4"/>
-      <c r="T6" s="7"/>
-      <c r="U6" s="6"/>
-      <c r="V6" s="7"/>
-      <c r="W6" s="7"/>
-      <c r="X6" s="7"/>
-      <c r="Y6" s="7"/>
-      <c r="Z6" s="7"/>
-    </row>
-    <row r="7" spans="1:26" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
-        <v>4</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="4">
-        <v>2</v>
-      </c>
-      <c r="E7" s="4">
-        <v>1</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+      <c r="E14" s="3">
         <v>5</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="4">
-        <v>4</v>
-      </c>
-      <c r="E8" s="4">
-        <v>2</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" s="4"/>
-    </row>
-    <row r="9" spans="1:26" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
-        <v>6</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="4">
-        <v>5</v>
-      </c>
-      <c r="E9" s="4">
-        <v>3</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="1:26" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
-        <v>7</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="4">
-        <v>4</v>
-      </c>
-      <c r="E10" s="4">
-        <v>3</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
-        <v>8</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="4">
-        <v>3</v>
-      </c>
-      <c r="E11" s="4">
-        <v>3</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
-        <v>9</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="4">
-        <v>5</v>
-      </c>
-      <c r="E12" s="4">
-        <v>4</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="G12" s="4"/>
-    </row>
-    <row r="13" spans="1:26" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
-        <v>10</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="4">
-        <v>2</v>
-      </c>
-      <c r="E13" s="4">
-        <v>4</v>
-      </c>
-      <c r="F13" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="G13" s="4"/>
-    </row>
-    <row r="14" spans="1:26" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
-        <v>11</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="4" t="s">
+      <c r="F14" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="G14" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="D14" s="4">
-        <v>1</v>
-      </c>
-      <c r="E14" s="4">
-        <v>5</v>
-      </c>
-      <c r="F14" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1282,7 +1272,7 @@
   <dimension ref="A1:P24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="X53" sqref="X53"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1295,365 +1285,365 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" s="9" t="s">
+      <c r="E3" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="12"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="J3" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="K3" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="L3" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="M3" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="N3" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="O3" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="P3" s="9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="13"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>1</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>1.5</v>
       </c>
-      <c r="D5" s="14"/>
+      <c r="D5" s="13"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B6" s="2">
+        <v>56</v>
+      </c>
+      <c r="B6" s="1">
         <v>1</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>1</v>
       </c>
-      <c r="D6" s="10" t="s">
-        <v>58</v>
+      <c r="D6" s="9" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>59</v>
-      </c>
-      <c r="B7" s="2">
+        <v>58</v>
+      </c>
+      <c r="B7" s="1">
         <v>1</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>2</v>
       </c>
-      <c r="D7" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="E7" s="10"/>
+      <c r="D7" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="9"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B8" s="2">
-        <v>1</v>
-      </c>
-      <c r="C8" s="2">
-        <v>1</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
       <c r="H9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>62</v>
-      </c>
-      <c r="B10" s="2">
+        <v>61</v>
+      </c>
+      <c r="B10" s="1">
         <v>3</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="1">
         <v>1</v>
       </c>
-      <c r="E10" s="12"/>
-      <c r="F10" s="10"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="9"/>
       <c r="H10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="2">
+        <v>16</v>
+      </c>
+      <c r="B11" s="1">
         <v>3</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="1">
         <v>2</v>
       </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
       <c r="H11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="2">
+        <v>8</v>
+      </c>
+      <c r="B12" s="1">
         <v>3</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="1">
         <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>58</v>
-      </c>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
+        <v>57</v>
+      </c>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="E13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="E13" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <v>5</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="1">
         <v>2</v>
       </c>
       <c r="E14" t="s">
-        <v>58</v>
-      </c>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
+        <v>57</v>
+      </c>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="2">
+        <v>20</v>
+      </c>
+      <c r="B15" s="1">
         <v>5</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="1">
         <v>2</v>
       </c>
-      <c r="H15" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="I15" s="10"/>
+      <c r="H15" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="I15" s="9"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
+      <c r="A16" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
       <c r="H16" t="s">
-        <v>58</v>
-      </c>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
+        <v>57</v>
+      </c>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>66</v>
-      </c>
-      <c r="B17" s="2">
+        <v>65</v>
+      </c>
+      <c r="B17" s="1">
         <v>7</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="1">
         <v>2</v>
       </c>
       <c r="H17" t="s">
-        <v>58</v>
-      </c>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="12"/>
+        <v>57</v>
+      </c>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>69</v>
-      </c>
-      <c r="B18" s="2">
+        <v>68</v>
+      </c>
+      <c r="B18" s="1">
         <v>8</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="1">
         <v>3</v>
       </c>
       <c r="H18" t="s">
-        <v>58</v>
-      </c>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="10"/>
+        <v>57</v>
+      </c>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>68</v>
-      </c>
-      <c r="B19" s="2">
+        <v>67</v>
+      </c>
+      <c r="B19" s="1">
         <v>9</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="1">
         <v>1</v>
       </c>
-      <c r="L19" s="10" t="s">
-        <v>58</v>
+      <c r="L19" s="9" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
+      <c r="A20" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
       <c r="K20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" s="2">
+        <v>29</v>
+      </c>
+      <c r="B21" s="1">
         <v>10</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="1">
         <v>2</v>
       </c>
       <c r="J21" t="s">
-        <v>58</v>
-      </c>
-      <c r="M21" s="10"/>
-      <c r="N21" s="10"/>
-      <c r="O21" s="12"/>
+        <v>57</v>
+      </c>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="11"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
+      <c r="A22" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
       <c r="J22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>71</v>
-      </c>
-      <c r="B23" s="2">
+        <v>70</v>
+      </c>
+      <c r="B23" s="1">
         <v>12</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="1">
         <v>2</v>
       </c>
       <c r="N23" t="s">
-        <v>58</v>
-      </c>
-      <c r="O23" s="10"/>
-      <c r="P23" s="10"/>
+        <v>57</v>
+      </c>
+      <c r="O23" s="9"/>
+      <c r="P23" s="9"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>72</v>
-      </c>
-      <c r="B24" s="2">
+        <v>71</v>
+      </c>
+      <c r="B24" s="1">
         <v>13</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="1">
         <v>1</v>
       </c>
       <c r="M24" t="s">
-        <v>58</v>
-      </c>
-      <c r="P24" s="10"/>
+        <v>57</v>
+      </c>
+      <c r="P24" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:H1"/>
   </mergeCells>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
   <tableParts count="2">

</xml_diff>